<commit_message>
Ophalen van Bijstands data. Closes #221. 👀 In Review
</commit_message>
<xml_diff>
--- a/src/main/resources/data/allecijfers/overzicht-nieuwegein.xlsx
+++ b/src/main/resources/data/allecijfers/overzicht-nieuwegein.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\IdeaProjects\LearnDiTwins\src\main\resources\data\allecijfers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CB8C2D-E530-4ADE-A71C-F945EFBB57B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A57D26-B9A8-4E4D-9C34-938D7FDBA1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="0" windowWidth="23835" windowHeight="21000" activeTab="4" xr2:uid="{50057F15-3147-432A-8EDA-956F5D835F7B}"/>
+    <workbookView xWindow="1320" yWindow="1140" windowWidth="21840" windowHeight="18495" activeTab="5" xr2:uid="{50057F15-3147-432A-8EDA-956F5D835F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="inwoneraantal" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Ouder dan 65" sheetId="2" r:id="rId3"/>
     <sheet name="huishouden" sheetId="3" r:id="rId4"/>
     <sheet name="bevolkinsdichtheid" sheetId="5" r:id="rId5"/>
+    <sheet name="bijstand" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="126">
   <si>
     <t>Leeftijd jonger dan 15 % Nieuwegein</t>
   </si>
@@ -415,6 +416,9 @@
   </si>
   <si>
     <t>Gemiddelde bevolkingsdichtheid Nieuwegein</t>
+  </si>
+  <si>
+    <t>Personen met bijstand % Nieuwegein</t>
   </si>
 </sst>
 </file>
@@ -10983,7 +10987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD9B471-9358-4BBF-8A5A-B2245D2AC499}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -13870,4 +13874,2733 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B576A26-99B8-42FE-9F67-00BBBBD30C90}">
+  <dimension ref="A1:N63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2013</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2014</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3">
+        <v>3.125E-2</v>
+      </c>
+      <c r="K2" s="3">
+        <v>2.7027027027027029E-2</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="M2" s="3">
+        <v>3.9735099337748353E-2</v>
+      </c>
+      <c r="N2" s="3">
+        <v>2.181818181818182E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>8.4388185654008432E-3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>6.993006993006993E-3</v>
+      </c>
+      <c r="K3" s="3">
+        <v>5.8823529411764714E-3</v>
+      </c>
+      <c r="L3" s="3">
+        <v>5.7471264367816091E-3</v>
+      </c>
+      <c r="M3" s="3">
+        <v>5.6980056980056983E-3</v>
+      </c>
+      <c r="N3" s="3">
+        <v>5.6338028169014088E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.1764705882352939E-2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1.4534883720930231E-2</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1.4492753623188409E-2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1.4450867052023119E-2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.4409221902017291E-2</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1.4598540145985399E-2</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1.461988304093568E-2</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1.167883211678832E-2</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1.282051282051282E-2</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1.2684989429175481E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.6129032258064519E-2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.810865191146881E-2</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2.014098690835851E-2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.9627085377821391E-2</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2.186878727634195E-2</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1.780415430267062E-2</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1.7612524461839529E-2</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1.7578125E-2</v>
+      </c>
+      <c r="M5" s="3">
+        <v>1.9398642095053351E-2</v>
+      </c>
+      <c r="N5" s="3">
+        <v>1.9047619047619049E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.510989010989011E-2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1.5099519560741251E-2</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.7918676774638181E-2</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2.0562028786840301E-2</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1.913875598086125E-2</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1.9230769230769228E-2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1.7711171662125338E-2</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1.9060585432266849E-2</v>
+      </c>
+      <c r="M6" s="3">
+        <v>3.6832412523020259E-3</v>
+      </c>
+      <c r="N6" s="3">
+        <v>3.7383177570093459E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.974183750949127E-2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.9908116385911181E-2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2.152190622598002E-2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>2.1472392638036811E-2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2.1571648690292759E-2</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1.9923371647509579E-2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1.9953952417498078E-2</v>
+      </c>
+      <c r="L7" s="3">
+        <v>1.984732824427481E-2</v>
+      </c>
+      <c r="M7" s="3">
+        <v>2.010827532869296E-2</v>
+      </c>
+      <c r="N7" s="3">
+        <v>2.0030816640986129E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3.1746031746031737E-2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3.669724770642202E-2</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2.9069767441860461E-2</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3.3519553072625698E-2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>3.39943342776204E-2</v>
+      </c>
+      <c r="J8" s="3">
+        <v>3.7940379403794043E-2</v>
+      </c>
+      <c r="K8" s="3">
+        <v>3.3519553072625698E-2</v>
+      </c>
+      <c r="L8" s="3">
+        <v>4.49438202247191E-2</v>
+      </c>
+      <c r="M8" s="3">
+        <v>3.825136612021858E-2</v>
+      </c>
+      <c r="N8" s="3">
+        <v>2.6595744680851061E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.6129032258064509E-2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1.810865191146881E-2</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2.014098690835851E-2</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1.9627085377821391E-2</v>
+      </c>
+      <c r="I9" s="3">
+        <v>2.186878727634195E-2</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1.780415430267062E-2</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1.7612524461839529E-2</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1.7578125E-2</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1.410934744268078E-2</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1.7391304347826091E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.2536679841293681E-2</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1.8915956400590069E-2</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1.9280506692521751E-2</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2.3721187149877788E-2</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1.7391304347826091E-2</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1.7492711370262391E-2</v>
+      </c>
+      <c r="K10" s="3">
+        <v>2.318840579710145E-2</v>
+      </c>
+      <c r="L10" s="3">
+        <v>2.318840579710145E-2</v>
+      </c>
+      <c r="M10" s="3">
+        <v>2.312138728323699E-2</v>
+      </c>
+      <c r="N10" s="3">
+        <v>2.3952095808383232E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.510989010989011E-2</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1.5099519560741251E-2</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1.7918676774638181E-2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2.0562028786840301E-2</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1.913875598086124E-2</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1.9230769230769228E-2</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1.7711171662125338E-2</v>
+      </c>
+      <c r="L11" s="3">
+        <v>1.9060585432266849E-2</v>
+      </c>
+      <c r="M11" s="3">
+        <v>1.778385772913817E-2</v>
+      </c>
+      <c r="N11" s="3">
+        <v>1.9257221458046769E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.0771992818671449E-2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.083032490974729E-2</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1.0714285714285709E-2</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1.058201058201058E-2</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1.0526315789473681E-2</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.029159519725557E-2</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1.018675721561969E-2</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1.0118043844856661E-2</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1.515151515151515E-2</v>
+      </c>
+      <c r="N12" s="3">
+        <v>1.503759398496241E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.6849199663016009E-2</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1.6792611251049541E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1.8518518518518521E-2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2.033898305084746E-2</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1.8612521150592219E-2</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1.8596787827557061E-2</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1.828761429758936E-2</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1.821192052980132E-2</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1.839464882943144E-2</v>
+      </c>
+      <c r="N13" s="3">
+        <v>1.658374792703151E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0.14736842105263159</v>
+      </c>
+      <c r="N14" s="3">
+        <v>9.6153846153846159E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.16666666666666671</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1.5384615384615391E-2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1.526717557251908E-2</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1.526717557251908E-2</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1.5748031496062988E-2</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1.5748031496062988E-2</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1.550387596899225E-2</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1.5873015873015869E-2</v>
+      </c>
+      <c r="L16" s="3">
+        <v>1.550387596899225E-2</v>
+      </c>
+      <c r="M16" s="3">
+        <v>1.5384615384615391E-2</v>
+      </c>
+      <c r="N16" s="3">
+        <v>1.5748031496062988E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1.6129032258064519E-2</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1.810865191146881E-2</v>
+      </c>
+      <c r="G17" s="3">
+        <v>2.014098690835851E-2</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1.9627085377821391E-2</v>
+      </c>
+      <c r="I17" s="3">
+        <v>2.186878727634195E-2</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1.780415430267062E-2</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1.7612524461839529E-2</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1.7578125E-2</v>
+      </c>
+      <c r="M17" s="3">
+        <v>2.159827213822894E-2</v>
+      </c>
+      <c r="N17" s="3">
+        <v>2.100840336134454E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1.6849199663016009E-2</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1.6792611251049541E-2</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1.8518518518518521E-2</v>
+      </c>
+      <c r="H18" s="3">
+        <v>2.033898305084746E-2</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1.8612521150592219E-2</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1.8596787827557061E-2</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1.828761429758936E-2</v>
+      </c>
+      <c r="L18" s="3">
+        <v>1.821192052980132E-2</v>
+      </c>
+      <c r="M18" s="3">
+        <v>1.7582417582417579E-2</v>
+      </c>
+      <c r="N18" s="3">
+        <v>1.7467248908296939E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3.8623005877413942E-2</v>
+      </c>
+      <c r="F19" s="3">
+        <v>4.3297252289758538E-2</v>
+      </c>
+      <c r="G19" s="3">
+        <v>4.5639771801141003E-2</v>
+      </c>
+      <c r="H19" s="3">
+        <v>4.5344129554655867E-2</v>
+      </c>
+      <c r="I19" s="3">
+        <v>4.5124899274778398E-2</v>
+      </c>
+      <c r="J19" s="3">
+        <v>4.49438202247191E-2</v>
+      </c>
+      <c r="K19" s="3">
+        <v>4.1500399042298478E-2</v>
+      </c>
+      <c r="L19" s="3">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="M19" s="3">
+        <v>3.6021926389976512E-2</v>
+      </c>
+      <c r="N19" s="3">
+        <v>3.7765538945712038E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1.1764705882352939E-2</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1.4534883720930231E-2</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1.4492753623188409E-2</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1.4450867052023119E-2</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1.4409221902017291E-2</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1.4598540145985399E-2</v>
+      </c>
+      <c r="K20" s="3">
+        <v>1.461988304093567E-2</v>
+      </c>
+      <c r="L20" s="3">
+        <v>1.167883211678832E-2</v>
+      </c>
+      <c r="M20" s="3">
+        <v>9.433962264150943E-3</v>
+      </c>
+      <c r="N20" s="3">
+        <v>9.3896713615023476E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1.974183750949127E-2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1.9908116385911181E-2</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2.152190622598002E-2</v>
+      </c>
+      <c r="H21" s="3">
+        <v>2.1472392638036811E-2</v>
+      </c>
+      <c r="I21" s="3">
+        <v>2.1571648690292759E-2</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1.9923371647509579E-2</v>
+      </c>
+      <c r="K21" s="3">
+        <v>1.9953952417498078E-2</v>
+      </c>
+      <c r="L21" s="3">
+        <v>1.984732824427481E-2</v>
+      </c>
+      <c r="M21" s="3">
+        <v>3.1847133757961783E-2</v>
+      </c>
+      <c r="N21" s="3">
+        <v>3.215434083601286E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0</v>
+      </c>
+      <c r="N22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3">
+        <v>0</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0.14736842105263159</v>
+      </c>
+      <c r="N23" s="3">
+        <v>9.6153846153846159E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1.974183750949127E-2</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1.9908116385911181E-2</v>
+      </c>
+      <c r="G24" s="3">
+        <v>2.1521906225980009E-2</v>
+      </c>
+      <c r="H24" s="3">
+        <v>2.1472392638036811E-2</v>
+      </c>
+      <c r="I24" s="3">
+        <v>2.1571648690292759E-2</v>
+      </c>
+      <c r="J24" s="3">
+        <v>1.9923371647509579E-2</v>
+      </c>
+      <c r="K24" s="3">
+        <v>1.9953952417498078E-2</v>
+      </c>
+      <c r="L24" s="3">
+        <v>1.984732824427481E-2</v>
+      </c>
+      <c r="M24" s="3">
+        <v>3.642987249544627E-3</v>
+      </c>
+      <c r="N24" s="3">
+        <v>3.610108303249098E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3">
+        <v>0</v>
+      </c>
+      <c r="N25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0.16666666666666671</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0</v>
+      </c>
+      <c r="N26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1.510989010989011E-2</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1.5099519560741251E-2</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1.7918676774638181E-2</v>
+      </c>
+      <c r="H27" s="3">
+        <v>2.0562028786840301E-2</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1.913875598086124E-2</v>
+      </c>
+      <c r="J27" s="3">
+        <v>1.9230769230769228E-2</v>
+      </c>
+      <c r="K27" s="3">
+        <v>1.7711171662125338E-2</v>
+      </c>
+      <c r="L27" s="3">
+        <v>1.9060585432266849E-2</v>
+      </c>
+      <c r="M27" s="3">
+        <v>3.6231884057971023E-2</v>
+      </c>
+      <c r="N27" s="3">
+        <v>3.9855072463768113E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0</v>
+      </c>
+      <c r="N28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="3">
+        <v>2.2883295194508008E-2</v>
+      </c>
+      <c r="F29" s="3">
+        <v>2.2624434389140271E-2</v>
+      </c>
+      <c r="G29" s="3">
+        <v>2.7210884353741499E-2</v>
+      </c>
+      <c r="H29" s="3">
+        <v>2.6966292134831461E-2</v>
+      </c>
+      <c r="I29" s="3">
+        <v>2.684563758389262E-2</v>
+      </c>
+      <c r="J29" s="3">
+        <v>2.2573363431151239E-2</v>
+      </c>
+      <c r="K29" s="3">
+        <v>2.714932126696833E-2</v>
+      </c>
+      <c r="L29" s="3">
+        <v>2.6966292134831461E-2</v>
+      </c>
+      <c r="M29" s="3">
+        <v>2.6258205689277898E-2</v>
+      </c>
+      <c r="N29" s="3">
+        <v>2.6258205689277898E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="3">
+        <v>1.8228097544954431E-2</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1.966085033177685E-2</v>
+      </c>
+      <c r="G30" s="3">
+        <v>2.1219639592582919E-2</v>
+      </c>
+      <c r="H30" s="3">
+        <v>2.2672431942217689E-2</v>
+      </c>
+      <c r="I30" s="3">
+        <v>2.3113725997284541E-2</v>
+      </c>
+      <c r="J30" s="3">
+        <v>2.1785794380546571E-2</v>
+      </c>
+      <c r="K30" s="3">
+        <v>2.094041500095184E-2</v>
+      </c>
+      <c r="L30" s="3">
+        <v>2.0642274116794299E-2</v>
+      </c>
+      <c r="M30" s="3">
+        <v>2.160774120815457E-2</v>
+      </c>
+      <c r="N30" s="3">
+        <v>2.0602906094122748E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1.974183750949127E-2</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1.9908116385911181E-2</v>
+      </c>
+      <c r="G31" s="3">
+        <v>2.152190622598002E-2</v>
+      </c>
+      <c r="H31" s="3">
+        <v>2.1472392638036811E-2</v>
+      </c>
+      <c r="I31" s="3">
+        <v>2.1571648690292759E-2</v>
+      </c>
+      <c r="J31" s="3">
+        <v>1.9923371647509579E-2</v>
+      </c>
+      <c r="K31" s="3">
+        <v>1.9953952417498078E-2</v>
+      </c>
+      <c r="L31" s="3">
+        <v>1.984732824427481E-2</v>
+      </c>
+      <c r="M31" s="3">
+        <v>3.2634032634032632E-2</v>
+      </c>
+      <c r="N31" s="3">
+        <v>3.2332563510392612E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
+        <v>0</v>
+      </c>
+      <c r="L32" s="3">
+        <v>0</v>
+      </c>
+      <c r="M32" s="3">
+        <v>0</v>
+      </c>
+      <c r="N32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="3">
+        <v>3.1746031746031737E-2</v>
+      </c>
+      <c r="F33" s="3">
+        <v>3.669724770642202E-2</v>
+      </c>
+      <c r="G33" s="3">
+        <v>2.9069767441860461E-2</v>
+      </c>
+      <c r="H33" s="3">
+        <v>3.3519553072625698E-2</v>
+      </c>
+      <c r="I33" s="3">
+        <v>3.39943342776204E-2</v>
+      </c>
+      <c r="J33" s="3">
+        <v>3.8043478260869568E-2</v>
+      </c>
+      <c r="K33" s="3">
+        <v>3.3613445378151259E-2</v>
+      </c>
+      <c r="L33" s="3">
+        <v>4.507042253521127E-2</v>
+      </c>
+      <c r="M33" s="3">
+        <v>3.8147138964577658E-2</v>
+      </c>
+      <c r="N33" s="3">
+        <v>2.6595744680851061E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3">
+        <v>3.125E-2</v>
+      </c>
+      <c r="K34" s="3">
+        <v>2.7027027027027029E-2</v>
+      </c>
+      <c r="L34" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="M34" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="N34" s="3">
+        <v>2.1739130434782612E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1.510989010989011E-2</v>
+      </c>
+      <c r="F35" s="3">
+        <v>1.5099519560741251E-2</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1.7918676774638181E-2</v>
+      </c>
+      <c r="H35" s="3">
+        <v>2.0562028786840301E-2</v>
+      </c>
+      <c r="I35" s="3">
+        <v>1.913875598086125E-2</v>
+      </c>
+      <c r="J35" s="3">
+        <v>1.9230769230769228E-2</v>
+      </c>
+      <c r="K35" s="3">
+        <v>1.7711171662125338E-2</v>
+      </c>
+      <c r="L35" s="3">
+        <v>1.9060585432266849E-2</v>
+      </c>
+      <c r="M35" s="3">
+        <v>1.6348773841961851E-2</v>
+      </c>
+      <c r="N35" s="3">
+        <v>1.08991825613079E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E36" s="3">
+        <v>9.4736842105263161E-2</v>
+      </c>
+      <c r="F36" s="3">
+        <v>8.6538461538461536E-2</v>
+      </c>
+      <c r="G36" s="3">
+        <v>9.2592592592592587E-2</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0.1071428571428571</v>
+      </c>
+      <c r="I36" s="3">
+        <v>9.5617529880478086E-2</v>
+      </c>
+      <c r="J36" s="3">
+        <v>7.6124567474048443E-2</v>
+      </c>
+      <c r="K36" s="3">
+        <v>6.8322981366459631E-2</v>
+      </c>
+      <c r="L36" s="3">
+        <v>6.7901234567901231E-2</v>
+      </c>
+      <c r="M36" s="3">
+        <v>6.2893081761006289E-2</v>
+      </c>
+      <c r="N36" s="3">
+        <v>6.1349693251533742E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1.0771992818671449E-2</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1.083032490974729E-2</v>
+      </c>
+      <c r="G37" s="3">
+        <v>1.0714285714285709E-2</v>
+      </c>
+      <c r="H37" s="3">
+        <v>1.058201058201058E-2</v>
+      </c>
+      <c r="I37" s="3">
+        <v>1.0526315789473681E-2</v>
+      </c>
+      <c r="J37" s="3">
+        <v>1.0291595197255581E-2</v>
+      </c>
+      <c r="K37" s="3">
+        <v>1.018675721561969E-2</v>
+      </c>
+      <c r="L37" s="3">
+        <v>1.0118043844856661E-2</v>
+      </c>
+      <c r="M37" s="3">
+        <v>1.2121212121212119E-2</v>
+      </c>
+      <c r="N37" s="3">
+        <v>1.201201201201201E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
+      <c r="J38" s="3">
+        <v>0</v>
+      </c>
+      <c r="K38" s="3">
+        <v>0</v>
+      </c>
+      <c r="L38" s="3">
+        <v>0</v>
+      </c>
+      <c r="M38" s="3">
+        <v>0</v>
+      </c>
+      <c r="N38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1.1764705882352939E-2</v>
+      </c>
+      <c r="F39" s="3">
+        <v>1.4534883720930231E-2</v>
+      </c>
+      <c r="G39" s="3">
+        <v>1.4492753623188409E-2</v>
+      </c>
+      <c r="H39" s="3">
+        <v>1.4450867052023119E-2</v>
+      </c>
+      <c r="I39" s="3">
+        <v>1.4409221902017291E-2</v>
+      </c>
+      <c r="J39" s="3">
+        <v>1.4598540145985399E-2</v>
+      </c>
+      <c r="K39" s="3">
+        <v>1.461988304093568E-2</v>
+      </c>
+      <c r="L39" s="3">
+        <v>1.167883211678832E-2</v>
+      </c>
+      <c r="M39" s="3">
+        <v>8.836524300441826E-3</v>
+      </c>
+      <c r="N39" s="3">
+        <v>8.7336244541484712E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="3">
+        <v>1.5384615384615391E-2</v>
+      </c>
+      <c r="F40" s="3">
+        <v>1.526717557251908E-2</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1.526717557251908E-2</v>
+      </c>
+      <c r="H40" s="3">
+        <v>1.5748031496062988E-2</v>
+      </c>
+      <c r="I40" s="3">
+        <v>1.5748031496062988E-2</v>
+      </c>
+      <c r="J40" s="3">
+        <v>1.550387596899225E-2</v>
+      </c>
+      <c r="K40" s="3">
+        <v>1.5873015873015869E-2</v>
+      </c>
+      <c r="L40" s="3">
+        <v>1.550387596899225E-2</v>
+      </c>
+      <c r="M40" s="3">
+        <v>1.5384615384615391E-2</v>
+      </c>
+      <c r="N40" s="3">
+        <v>1.5748031496062988E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
+      <c r="I41" s="3">
+        <v>0</v>
+      </c>
+      <c r="J41" s="3">
+        <v>0</v>
+      </c>
+      <c r="K41" s="3">
+        <v>0</v>
+      </c>
+      <c r="L41" s="3">
+        <v>0</v>
+      </c>
+      <c r="M41" s="3">
+        <v>0</v>
+      </c>
+      <c r="N41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" s="3">
+        <v>9.4736842105263161E-2</v>
+      </c>
+      <c r="F42" s="3">
+        <v>8.6538461538461536E-2</v>
+      </c>
+      <c r="G42" s="3">
+        <v>9.2592592592592587E-2</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0.1071428571428571</v>
+      </c>
+      <c r="I42" s="3">
+        <v>9.5617529880478086E-2</v>
+      </c>
+      <c r="J42" s="3">
+        <v>7.586206896551724E-2</v>
+      </c>
+      <c r="K42" s="3">
+        <v>6.8111455108359129E-2</v>
+      </c>
+      <c r="L42" s="3">
+        <v>6.7901234567901231E-2</v>
+      </c>
+      <c r="M42" s="3">
+        <v>6.2695924764890276E-2</v>
+      </c>
+      <c r="N42" s="3">
+        <v>6.1349693251533742E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" s="3">
+        <v>6.9204152249134942E-3</v>
+      </c>
+      <c r="F43" s="3">
+        <v>6.9767441860465124E-3</v>
+      </c>
+      <c r="G43" s="3">
+        <v>7.0298769771529003E-3</v>
+      </c>
+      <c r="H43" s="3">
+        <v>9.3676814988290415E-3</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1.0613207547169811E-2</v>
+      </c>
+      <c r="J43" s="3">
+        <v>1.070791195716835E-2</v>
+      </c>
+      <c r="K43" s="3">
+        <v>9.5522388059701493E-3</v>
+      </c>
+      <c r="L43" s="3">
+        <v>9.5693779904306216E-3</v>
+      </c>
+      <c r="M43" s="3">
+        <v>1.3179571663920919E-2</v>
+      </c>
+      <c r="N43" s="3">
+        <v>1.3311148086522459E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="3">
+        <v>1.6849199663016009E-2</v>
+      </c>
+      <c r="F44" s="3">
+        <v>1.6792611251049541E-2</v>
+      </c>
+      <c r="G44" s="3">
+        <v>1.8518518518518521E-2</v>
+      </c>
+      <c r="H44" s="3">
+        <v>2.033898305084746E-2</v>
+      </c>
+      <c r="I44" s="3">
+        <v>1.8612521150592219E-2</v>
+      </c>
+      <c r="J44" s="3">
+        <v>1.8596787827557061E-2</v>
+      </c>
+      <c r="K44" s="3">
+        <v>1.828761429758936E-2</v>
+      </c>
+      <c r="L44" s="3">
+        <v>1.821192052980132E-2</v>
+      </c>
+      <c r="M44" s="3">
+        <v>1.7505470459518599E-2</v>
+      </c>
+      <c r="N44" s="3">
+        <v>1.284796573875803E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1.951951951951952E-2</v>
+      </c>
+      <c r="F45" s="3">
+        <v>1.963746223564955E-2</v>
+      </c>
+      <c r="G45" s="3">
+        <v>2.1148036253776429E-2</v>
+      </c>
+      <c r="H45" s="3">
+        <v>2.4260803639120549E-2</v>
+      </c>
+      <c r="I45" s="3">
+        <v>2.5855513307984791E-2</v>
+      </c>
+      <c r="J45" s="3">
+        <v>2.7522935779816519E-2</v>
+      </c>
+      <c r="K45" s="3">
+        <v>2.4672320740169621E-2</v>
+      </c>
+      <c r="L45" s="3">
+        <v>2.2935779816513759E-2</v>
+      </c>
+      <c r="M45" s="3">
+        <v>1.7699115044247791E-2</v>
+      </c>
+      <c r="N45" s="3">
+        <v>1.754385964912281E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46" s="3">
+        <v>3.8623005877413942E-2</v>
+      </c>
+      <c r="F46" s="3">
+        <v>4.3297252289758531E-2</v>
+      </c>
+      <c r="G46" s="3">
+        <v>4.5639771801141003E-2</v>
+      </c>
+      <c r="H46" s="3">
+        <v>4.5344129554655867E-2</v>
+      </c>
+      <c r="I46" s="3">
+        <v>4.5124899274778398E-2</v>
+      </c>
+      <c r="J46" s="3">
+        <v>4.4943820224719107E-2</v>
+      </c>
+      <c r="K46" s="3">
+        <v>4.1500399042298478E-2</v>
+      </c>
+      <c r="L46" s="3">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="M46" s="3">
+        <v>2.551020408163265E-2</v>
+      </c>
+      <c r="N46" s="3">
+        <v>2.538071065989848E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E47" s="3">
+        <v>6.920415224913495E-3</v>
+      </c>
+      <c r="F47" s="3">
+        <v>6.9767441860465124E-3</v>
+      </c>
+      <c r="G47" s="3">
+        <v>7.0298769771528994E-3</v>
+      </c>
+      <c r="H47" s="3">
+        <v>9.3676814988290415E-3</v>
+      </c>
+      <c r="I47" s="3">
+        <v>1.0613207547169811E-2</v>
+      </c>
+      <c r="J47" s="3">
+        <v>1.070791195716835E-2</v>
+      </c>
+      <c r="K47" s="3">
+        <v>9.5522388059701493E-3</v>
+      </c>
+      <c r="L47" s="3">
+        <v>9.5693779904306234E-3</v>
+      </c>
+      <c r="M47" s="3">
+        <v>7.0671378091872791E-3</v>
+      </c>
+      <c r="N47" s="3">
+        <v>7.2072072072072073E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" s="3">
+        <v>3.8623005877413942E-2</v>
+      </c>
+      <c r="F48" s="3">
+        <v>4.3297252289758531E-2</v>
+      </c>
+      <c r="G48" s="3">
+        <v>4.5639771801141003E-2</v>
+      </c>
+      <c r="H48" s="3">
+        <v>4.5344129554655867E-2</v>
+      </c>
+      <c r="I48" s="3">
+        <v>4.5124899274778398E-2</v>
+      </c>
+      <c r="J48" s="3">
+        <v>4.4943820224719107E-2</v>
+      </c>
+      <c r="K48" s="3">
+        <v>4.1500399042298478E-2</v>
+      </c>
+      <c r="L48" s="3">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="M48" s="3">
+        <v>5.7761732851985562E-2</v>
+      </c>
+      <c r="N48" s="3">
+        <v>6.1705989110707807E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" s="3">
+        <v>6.920415224913495E-3</v>
+      </c>
+      <c r="F49" s="3">
+        <v>6.9767441860465124E-3</v>
+      </c>
+      <c r="G49" s="3">
+        <v>7.0298769771529003E-3</v>
+      </c>
+      <c r="H49" s="3">
+        <v>9.3676814988290398E-3</v>
+      </c>
+      <c r="I49" s="3">
+        <v>1.0613207547169811E-2</v>
+      </c>
+      <c r="J49" s="3">
+        <v>1.070791195716835E-2</v>
+      </c>
+      <c r="K49" s="3">
+        <v>9.5522388059701476E-3</v>
+      </c>
+      <c r="L49" s="3">
+        <v>9.5693779904306216E-3</v>
+      </c>
+      <c r="M49" s="3">
+        <v>0</v>
+      </c>
+      <c r="N49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1.2536679841293681E-2</v>
+      </c>
+      <c r="F50" s="3">
+        <v>1.8915956400590069E-2</v>
+      </c>
+      <c r="G50" s="3">
+        <v>1.9280506692521751E-2</v>
+      </c>
+      <c r="H50" s="3">
+        <v>2.3721187149877788E-2</v>
+      </c>
+      <c r="I50" s="3">
+        <v>1.7391304347826091E-2</v>
+      </c>
+      <c r="J50" s="3">
+        <v>1.7492711370262391E-2</v>
+      </c>
+      <c r="K50" s="3">
+        <v>2.3255813953488368E-2</v>
+      </c>
+      <c r="L50" s="3">
+        <v>2.312138728323699E-2</v>
+      </c>
+      <c r="M50" s="3">
+        <v>2.3054755043227661E-2</v>
+      </c>
+      <c r="N50" s="3">
+        <v>2.3952095808383232E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" s="3">
+        <v>2.2883295194508008E-2</v>
+      </c>
+      <c r="F51" s="3">
+        <v>2.2624434389140271E-2</v>
+      </c>
+      <c r="G51" s="3">
+        <v>2.7210884353741499E-2</v>
+      </c>
+      <c r="H51" s="3">
+        <v>2.6966292134831461E-2</v>
+      </c>
+      <c r="I51" s="3">
+        <v>2.684563758389262E-2</v>
+      </c>
+      <c r="J51" s="3">
+        <v>2.2573363431151239E-2</v>
+      </c>
+      <c r="K51" s="3">
+        <v>2.714932126696833E-2</v>
+      </c>
+      <c r="L51" s="3">
+        <v>2.6966292134831461E-2</v>
+      </c>
+      <c r="M51" s="3">
+        <v>2.6258205689277898E-2</v>
+      </c>
+      <c r="N51" s="3">
+        <v>2.6258205689277898E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1.0771992818671449E-2</v>
+      </c>
+      <c r="F52" s="3">
+        <v>1.083032490974729E-2</v>
+      </c>
+      <c r="G52" s="3">
+        <v>1.0714285714285709E-2</v>
+      </c>
+      <c r="H52" s="3">
+        <v>1.058201058201058E-2</v>
+      </c>
+      <c r="I52" s="3">
+        <v>1.0526315789473681E-2</v>
+      </c>
+      <c r="J52" s="3">
+        <v>1.0291595197255581E-2</v>
+      </c>
+      <c r="K52" s="3">
+        <v>1.01867572156197E-2</v>
+      </c>
+      <c r="L52" s="3">
+        <v>1.0118043844856661E-2</v>
+      </c>
+      <c r="M52" s="3">
+        <v>1.3468013468013469E-2</v>
+      </c>
+      <c r="N52" s="3">
+        <v>1.003344481605351E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1.951951951951952E-2</v>
+      </c>
+      <c r="F53" s="3">
+        <v>1.963746223564955E-2</v>
+      </c>
+      <c r="G53" s="3">
+        <v>2.1148036253776439E-2</v>
+      </c>
+      <c r="H53" s="3">
+        <v>2.4260803639120549E-2</v>
+      </c>
+      <c r="I53" s="3">
+        <v>2.5855513307984791E-2</v>
+      </c>
+      <c r="J53" s="3">
+        <v>2.7522935779816508E-2</v>
+      </c>
+      <c r="K53" s="3">
+        <v>2.4672320740169621E-2</v>
+      </c>
+      <c r="L53" s="3">
+        <v>2.2935779816513759E-2</v>
+      </c>
+      <c r="M53" s="3">
+        <v>2.279202279202279E-2</v>
+      </c>
+      <c r="N53" s="3">
+        <v>1.734104046242774E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1.6849199663016009E-2</v>
+      </c>
+      <c r="F54" s="3">
+        <v>1.6792611251049541E-2</v>
+      </c>
+      <c r="G54" s="3">
+        <v>1.8518518518518521E-2</v>
+      </c>
+      <c r="H54" s="3">
+        <v>2.033898305084746E-2</v>
+      </c>
+      <c r="I54" s="3">
+        <v>1.8612521150592219E-2</v>
+      </c>
+      <c r="J54" s="3">
+        <v>1.8596787827557061E-2</v>
+      </c>
+      <c r="K54" s="3">
+        <v>1.828761429758936E-2</v>
+      </c>
+      <c r="L54" s="3">
+        <v>1.821192052980132E-2</v>
+      </c>
+      <c r="M54" s="3">
+        <v>2.1126760563380281E-2</v>
+      </c>
+      <c r="N54" s="3">
+        <v>2.1352313167259791E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1.951951951951952E-2</v>
+      </c>
+      <c r="F55" s="3">
+        <v>1.9637462235649539E-2</v>
+      </c>
+      <c r="G55" s="3">
+        <v>2.1148036253776429E-2</v>
+      </c>
+      <c r="H55" s="3">
+        <v>2.4260803639120539E-2</v>
+      </c>
+      <c r="I55" s="3">
+        <v>2.5855513307984791E-2</v>
+      </c>
+      <c r="J55" s="3">
+        <v>2.7522935779816508E-2</v>
+      </c>
+      <c r="K55" s="3">
+        <v>2.4672320740169621E-2</v>
+      </c>
+      <c r="L55" s="3">
+        <v>2.2935779816513759E-2</v>
+      </c>
+      <c r="M55" s="3">
+        <v>2.922077922077922E-2</v>
+      </c>
+      <c r="N55" s="3">
+        <v>2.61437908496732E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3">
+        <v>0</v>
+      </c>
+      <c r="G56" s="3">
+        <v>0</v>
+      </c>
+      <c r="H56" s="3">
+        <v>0</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0</v>
+      </c>
+      <c r="J56" s="3">
+        <v>0</v>
+      </c>
+      <c r="K56" s="3">
+        <v>0</v>
+      </c>
+      <c r="L56" s="3">
+        <v>0</v>
+      </c>
+      <c r="M56" s="3">
+        <v>0</v>
+      </c>
+      <c r="N56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57" s="3">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3">
+        <v>0</v>
+      </c>
+      <c r="G57" s="3">
+        <v>0</v>
+      </c>
+      <c r="H57" s="3">
+        <v>0</v>
+      </c>
+      <c r="I57" s="3">
+        <v>0</v>
+      </c>
+      <c r="J57" s="3">
+        <v>0</v>
+      </c>
+      <c r="K57" s="3">
+        <v>0</v>
+      </c>
+      <c r="L57" s="3">
+        <v>0</v>
+      </c>
+      <c r="M57" s="3">
+        <v>0</v>
+      </c>
+      <c r="N57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E58" s="3">
+        <v>6.9204152249134959E-3</v>
+      </c>
+      <c r="F58" s="3">
+        <v>6.9767441860465124E-3</v>
+      </c>
+      <c r="G58" s="3">
+        <v>7.0298769771528994E-3</v>
+      </c>
+      <c r="H58" s="3">
+        <v>9.3676814988290415E-3</v>
+      </c>
+      <c r="I58" s="3">
+        <v>1.0613207547169811E-2</v>
+      </c>
+      <c r="J58" s="3">
+        <v>1.070791195716835E-2</v>
+      </c>
+      <c r="K58" s="3">
+        <v>9.5522388059701493E-3</v>
+      </c>
+      <c r="L58" s="3">
+        <v>9.5693779904306234E-3</v>
+      </c>
+      <c r="M58" s="3">
+        <v>8.4084084084084087E-3</v>
+      </c>
+      <c r="N58" s="3">
+        <v>9.7739767868051317E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="3">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3">
+        <v>8.4388185654008432E-3</v>
+      </c>
+      <c r="G59" s="3">
+        <v>0</v>
+      </c>
+      <c r="H59" s="3">
+        <v>0</v>
+      </c>
+      <c r="I59" s="3">
+        <v>0</v>
+      </c>
+      <c r="J59" s="3">
+        <v>6.9686411149825784E-3</v>
+      </c>
+      <c r="K59" s="3">
+        <v>5.8997050147492616E-3</v>
+      </c>
+      <c r="L59" s="3">
+        <v>5.7471264367816091E-3</v>
+      </c>
+      <c r="M59" s="3">
+        <v>5.681818181818182E-3</v>
+      </c>
+      <c r="N59" s="3">
+        <v>5.6338028169014088E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E60" s="3">
+        <v>3.8623005877413942E-2</v>
+      </c>
+      <c r="F60" s="3">
+        <v>4.3297252289758531E-2</v>
+      </c>
+      <c r="G60" s="3">
+        <v>4.5639771801141003E-2</v>
+      </c>
+      <c r="H60" s="3">
+        <v>4.5344129554655867E-2</v>
+      </c>
+      <c r="I60" s="3">
+        <v>4.5124899274778411E-2</v>
+      </c>
+      <c r="J60" s="3">
+        <v>4.49438202247191E-2</v>
+      </c>
+      <c r="K60" s="3">
+        <v>4.1500399042298478E-2</v>
+      </c>
+      <c r="L60" s="3">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="M60" s="3">
+        <v>1.204819277108434E-2</v>
+      </c>
+      <c r="N60" s="3">
+        <v>1.226993865030675E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61" s="3">
+        <v>6.920415224913495E-3</v>
+      </c>
+      <c r="F61" s="3">
+        <v>6.9767441860465124E-3</v>
+      </c>
+      <c r="G61" s="3">
+        <v>7.0298769771529003E-3</v>
+      </c>
+      <c r="H61" s="3">
+        <v>9.3676814988290398E-3</v>
+      </c>
+      <c r="I61" s="3">
+        <v>1.0613207547169811E-2</v>
+      </c>
+      <c r="J61" s="3">
+        <v>1.070791195716835E-2</v>
+      </c>
+      <c r="K61" s="3">
+        <v>9.5522388059701493E-3</v>
+      </c>
+      <c r="L61" s="3">
+        <v>9.5693779904306234E-3</v>
+      </c>
+      <c r="M61" s="3">
+        <v>8.23045267489712E-3</v>
+      </c>
+      <c r="N61" s="3">
+        <v>8.4210526315789472E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E62" s="3">
+        <v>0</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3">
+        <v>0</v>
+      </c>
+      <c r="H62" s="3">
+        <v>0</v>
+      </c>
+      <c r="I62" s="3">
+        <v>0</v>
+      </c>
+      <c r="J62" s="3">
+        <v>0</v>
+      </c>
+      <c r="K62" s="3">
+        <v>0</v>
+      </c>
+      <c r="L62" s="3">
+        <v>0</v>
+      </c>
+      <c r="M62" s="3">
+        <v>0</v>
+      </c>
+      <c r="N62" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E63" s="3">
+        <v>1.951951951951952E-2</v>
+      </c>
+      <c r="F63" s="3">
+        <v>1.963746223564955E-2</v>
+      </c>
+      <c r="G63" s="3">
+        <v>2.1148036253776439E-2</v>
+      </c>
+      <c r="H63" s="3">
+        <v>2.4260803639120549E-2</v>
+      </c>
+      <c r="I63" s="3">
+        <v>2.5855513307984791E-2</v>
+      </c>
+      <c r="J63" s="3">
+        <v>2.7522935779816519E-2</v>
+      </c>
+      <c r="K63" s="3">
+        <v>2.4672320740169621E-2</v>
+      </c>
+      <c r="L63" s="3">
+        <v>2.2935779816513759E-2</v>
+      </c>
+      <c r="M63" s="3">
+        <v>2.298850574712644E-2</v>
+      </c>
+      <c r="N63" s="3">
+        <v>2.152190622598002E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>